<commit_message>
After MR instrument entry
</commit_message>
<xml_diff>
--- a/Momentum Reversal Instrument Details.xlsx
+++ b/Momentum Reversal Instrument Details.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Instrument Name</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>ADANIENT</t>
-  </si>
-  <si>
-    <t>dsdsd</t>
   </si>
 </sst>
 </file>
@@ -388,7 +385,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -420,19 +417,22 @@
       <c r="B2" t="b">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
+      <c r="D2">
+        <v>2250</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
+      <c r="B3" t="b">
+        <v>1</v>
+      </c>
       <c r="C3" t="b">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>2222</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Before candle stick timeframe bug fix
</commit_message>
<xml_diff>
--- a/Momentum Reversal Instrument Details.xlsx
+++ b/Momentum Reversal Instrument Details.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\algo2trade\Code\Algo2Trade Live\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="22980" windowHeight="9555"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,8 +47,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,8 +97,44 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -140,7 +181,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -172,9 +213,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -206,6 +248,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -381,19 +424,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -410,7 +453,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -421,7 +464,7 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -442,24 +485,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>